<commit_message>
Update employee and patient example files with new data
</commit_message>
<xml_diff>
--- a/example_import_files/employee_examples.xlsx
+++ b/example_import_files/employee_examples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markj/Documents/Studium/Master Maschinenbau TH Koeln/Digitalisierung/SAPV_route_optimization/example_import_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE8C4DA-125C-8B4F-BD86-93858F47D20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558D0A7C-FE6D-E744-B8D4-2A9F9D3FC723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2980" yWindow="2220" windowWidth="28240" windowHeight="17240" xr2:uid="{BE61D418-1F51-B847-91F0-443E93710B5C}"/>
   </bookViews>
@@ -85,9 +85,6 @@
     <t>Wagner</t>
   </si>
   <si>
-    <t>Kirchplatz 3</t>
-  </si>
-  <si>
     <t>Wiehl</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>Klein</t>
   </si>
   <si>
-    <t>Talweg 7</t>
-  </si>
-  <si>
     <t>Petra</t>
   </si>
   <si>
@@ -130,35 +124,41 @@
     <t>Müller</t>
   </si>
   <si>
-    <t>Kaiserstraße 10</t>
-  </si>
-  <si>
-    <t>Bahnhofstraße 5</t>
-  </si>
-  <si>
     <t>Wipperfürth</t>
   </si>
   <si>
-    <t>Hauptstraße 20</t>
-  </si>
-  <si>
-    <t>Dorfstraße 15</t>
-  </si>
-  <si>
-    <t>Marktstraße 8</t>
-  </si>
-  <si>
-    <t>Bergstraße 25</t>
-  </si>
-  <si>
-    <t>Wiesenstraße 18</t>
+    <t>Hindenburgstraße 6</t>
+  </si>
+  <si>
+    <t>Moltkestraße 10</t>
+  </si>
+  <si>
+    <t>Breiter Weg 19</t>
+  </si>
+  <si>
+    <t>Lüdenscheider Straße 8</t>
+  </si>
+  <si>
+    <t>Weiherplatz 7</t>
+  </si>
+  <si>
+    <t>Ringstraße 22</t>
+  </si>
+  <si>
+    <t>Kölner Straße 33</t>
+  </si>
+  <si>
+    <t>Marktstraße 5</t>
+  </si>
+  <si>
+    <t>Homburger Straße 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -293,6 +293,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -475,7 +483,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -590,6 +598,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -640,8 +663,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1021,7 +1044,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1053,232 +1076,232 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2">
         <v>51643</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="2">
-        <v>51645</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3">
+        <v>51643</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4">
         <v>51647</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4">
         <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5">
         <v>51688</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6">
+        <v>51674</v>
+      </c>
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="2">
-        <v>51674</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6">
         <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="2">
-        <v>51643</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7">
+        <v>51645</v>
+      </c>
+      <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7">
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="D8">
         <v>51645</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8">
         <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9">
         <v>51647</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10">
         <v>51688</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11">
         <v>51674</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update example import files with new data
</commit_message>
<xml_diff>
--- a/example_import_files/employee_examples.xlsx
+++ b/example_import_files/employee_examples.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markj/Documents/Studium/Master Maschinenbau TH Koeln/Digitalisierung/SAPV_route_optimization/example_import_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558D0A7C-FE6D-E744-B8D4-2A9F9D3FC723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D613B33-1F88-6543-AA2A-29E06EA1A35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2980" yWindow="2220" windowWidth="28240" windowHeight="17240" xr2:uid="{BE61D418-1F51-B847-91F0-443E93710B5C}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>Vorname</t>
   </si>
@@ -133,18 +133,9 @@
     <t>Moltkestraße 10</t>
   </si>
   <si>
-    <t>Breiter Weg 19</t>
-  </si>
-  <si>
     <t>Lüdenscheider Straße 8</t>
   </si>
   <si>
-    <t>Weiherplatz 7</t>
-  </si>
-  <si>
-    <t>Ringstraße 22</t>
-  </si>
-  <si>
     <t>Kölner Straße 33</t>
   </si>
   <si>
@@ -152,6 +143,18 @@
   </si>
   <si>
     <t>Homburger Straße 2</t>
+  </si>
+  <si>
+    <t>Breiter Weg 21</t>
+  </si>
+  <si>
+    <t>Weiherplatz 15</t>
+  </si>
+  <si>
+    <t>Florastraße 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wiehl</t>
   </si>
 </sst>
 </file>
@@ -1044,7 +1047,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1129,7 +1132,7 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D4">
         <v>51647</v>
@@ -1152,7 +1155,7 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5">
         <v>51688</v>
@@ -1175,7 +1178,7 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D6">
         <v>51674</v>
@@ -1198,13 +1201,13 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D7">
-        <v>51645</v>
+        <v>51674</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -1244,7 +1247,7 @@
         <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D9">
         <v>51647</v>
@@ -1267,7 +1270,7 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D10">
         <v>51688</v>
@@ -1290,7 +1293,7 @@
         <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D11">
         <v>51674</v>

</xml_diff>

<commit_message>
Standardize visit type and function abbreviations across application
</commit_message>
<xml_diff>
--- a/example_import_files/employee_examples.xlsx
+++ b/example_import_files/employee_examples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markj/Documents/Studium/Master Maschinenbau TH Koeln/Digitalisierung/SAPV_route_optimization/example_import_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D613B33-1F88-6543-AA2A-29E06EA1A35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DB41AC-8823-8740-B152-28070D5DBB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2980" yWindow="2220" windowWidth="28240" windowHeight="17240" xr2:uid="{BE61D418-1F51-B847-91F0-443E93710B5C}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
   <si>
     <t>Vorname</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Wiehl</t>
+  </si>
+  <si>
+    <t>PDL</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1050,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1210,7 +1213,7 @@
         <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="G7">
         <v>100</v>

</xml_diff>